<commit_message>
Added logic to the rest of the buttons, except for the last one
</commit_message>
<xml_diff>
--- a/Family_lists.xlsx
+++ b/Family_lists.xlsx
@@ -1,38 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hitar\source\Family_tree\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Креховецьких" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Попич" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Test" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,21 +49,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -331,13 +388,544 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8.85546875" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>D:/_krekhovetskyi_/Я/20191227125653_IMG_2696.png</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>КА2000ТТ1995</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>КМ1960ПГ1971</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>КА2000</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Чоловіча</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Креховецький</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Андрій</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Миронович</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>с. Витвиця</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>КІ1994КЛ1996</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>КМ1960ПГ1971</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>КІ1994</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Чоловіча</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Креховецький</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Ігор</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Миронович</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1994</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>КІ1994КЛ1996</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>КЛ1996</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Жіноча</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Курило-Круховецька</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Любов</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ігорівна</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1996</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>КІ1994КЛ1996</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>КВ2017</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Чоловіча</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Креховецький</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Віталій </t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ігорович</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>КА2000ТТ1995</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ТТ1995</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Жіноча</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Тестовецька</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Тест</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1995</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>КМ1960ПГ1971</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>КМ1960</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Чоловіча</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Креховецький</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Мирон </t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Іванович</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>КМ1960ПГ1971</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ПГ1971</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Жіноча</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">П'єлик-Креховецька </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Галин</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Павлівна</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1971</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>КТ1990</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Чоловіча</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Креховецькпий</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Тестовий </t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Брат</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>КА2000ТТ1995</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ТД2005</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Жіноча</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Тестова </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ДИТИНА</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ТБ2001</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Чоловіча</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Тестовий Брат</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Брат</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>D:/_krekhovetskyi_/Природа/Перший дзвоник 11 клас, 2017/IMG_20170901_201604.jpg</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ПЛ2001</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Жіноча</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Попич</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Лідія</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ПЛ0000</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Жіноча</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Попич</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Лариса</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0000</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>